<commit_message>
bug fix for LTC
</commit_message>
<xml_diff>
--- a/EvoTax.1099/wwwroot/Templates/Form1099_PATR_Template.xlsx
+++ b/EvoTax.1099/wwwroot/Templates/Form1099_PATR_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://matthewjohnmcnally-my.sharepoint.com/personal/obaig_evolvedtax_com/Documents/Desktop/Excel sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Code Repos\EvoTaxes\EvoTax.1099\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_2860C95448794993C19DC1B8B86D6C480DDAF930" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22D9FA56-1073-49FD-AD36-A31EC877EF0C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC5DADB-0AD2-412F-8A84-7989B7456A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="149">
   <si>
     <t>Rcp TIN</t>
   </si>
@@ -464,10 +464,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Is Corrected</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Is Corrected Form of 1099</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1103,20 @@
     </xf>
     <xf numFmtId="49" fontId="22" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1121,19 +1134,6 @@
     <xf numFmtId="0" fontId="21" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1459,7 +1459,7 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2:AF12"/>
+      <selection activeCell="AF9" sqref="AF9:AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1581,8 +1581,8 @@
       <c r="AE1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="22" t="s">
-        <v>147</v>
+      <c r="AF1" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
@@ -1635,7 +1635,7 @@
         <v>38</v>
       </c>
       <c r="AF2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
@@ -1691,7 +1691,7 @@
         <v>37</v>
       </c>
       <c r="AF3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
@@ -1756,7 +1756,7 @@
         <v>37</v>
       </c>
       <c r="AF4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
@@ -1821,7 +1821,7 @@
         <v>37</v>
       </c>
       <c r="AF5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
@@ -1865,7 +1865,7 @@
         <v>37</v>
       </c>
       <c r="AF6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -1921,7 +1921,7 @@
         <v>37</v>
       </c>
       <c r="AF7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.35">
@@ -1971,7 +1971,7 @@
         <v>37</v>
       </c>
       <c r="AF8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.35">
@@ -2048,7 +2048,7 @@
         <v>44</v>
       </c>
       <c r="AF9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
@@ -2110,7 +2110,7 @@
         <v>37</v>
       </c>
       <c r="AF10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.35">
@@ -2160,7 +2160,7 @@
         <v>37</v>
       </c>
       <c r="AF11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
@@ -2210,7 +2210,7 @@
         <v>37</v>
       </c>
       <c r="AF12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.35">
@@ -2267,6 +2267,9 @@
       </c>
       <c r="AC13" t="s">
         <v>37</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2293,201 +2296,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="7" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="7" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="21"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="21"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A6:K6"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="A8:K8"/>
@@ -2496,12 +2505,6 @@
     <mergeCell ref="A11:K11"/>
     <mergeCell ref="A12:K12"/>
     <mergeCell ref="A13:K13"/>
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A6:K6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>